<commit_message>
Added 10125 and 10126.sah to SFM Search test-cases
Added 10125 and 10126.sah to SFM Search test-cases
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/backOffice/bo_excleData/SFMSearchDatasheet.xlsx
+++ b/svmx/test_lab/test_cases/backOffice/bo_excleData/SFMSearchDatasheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghanarao/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/sahi_pro/userdata/scripts/Sahi_Project/svmx/test_lab/test_cases/backOffice/bo_excleData/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="15740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,154 +27,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>CreateWorkOrder</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF3933FF"/>
-        <rFont val="Monaco"/>
-      </rPr>
-      <t>SVMXC__Service_Order__c  WO = new SVMXC__Service_Order__c ( SVMXC__Company__c ='"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Monaco"/>
-      </rPr>
-      <t>+ $Account2 +</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF3933FF"/>
-        <rFont val="Monaco"/>
-      </rPr>
-      <t>"', SVMXC__Product__c = '"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Monaco"/>
-      </rPr>
-      <t>+$Product+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF3933FF"/>
-        <rFont val="Monaco"/>
-      </rPr>
-      <t>"' , SVMXC__Group_Member__c = '"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Monaco"/>
-      </rPr>
-      <t>+$Technician+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF3933FF"/>
-        <rFont val="Monaco"/>
-      </rPr>
-      <t>"' ,SVMXC__Component__c = '"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Monaco"/>
-      </rPr>
-      <t>+$Component+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF3933FF"/>
-        <rFont val="Monaco"/>
-      </rPr>
-      <t>"',SVMXC__Order_Status__c = '"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Monaco"/>
-      </rPr>
-      <t>+$OrderStatus+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF3933FF"/>
-        <rFont val="Monaco"/>
-      </rPr>
-      <t>"' , SVMXC__Closed_On__c = "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Monaco"/>
-      </rPr>
-      <t>+$Closedon+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF3933FF"/>
-        <rFont val="Monaco"/>
-      </rPr>
-      <t>",SVMXC__Country__c = 'United States', SVMXC__Sub_Status__c = 'Resolved', SVMXC__Priority__c = 'High', SVMXC__Site__c = '"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Monaco"/>
-      </rPr>
-      <t>+$Site+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF3933FF"/>
-        <rFont val="Monaco"/>
-      </rPr>
-      <t>"', SVMXC__Scheduled_Date__c = Date.valueOf('"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Monaco"/>
-      </rPr>
-      <t>+$ScheduledDate+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF3933FF"/>
-        <rFont val="Monaco"/>
-      </rPr>
-      <t>"') );insert WO;</t>
-    </r>
+    <t>fetchwo</t>
+  </si>
+  <si>
+    <t>Select Name , Id from SVMXC__Service_Order__c where Createdby.Id = '005q0000003GGfP' Order by CreatedDate DESC Limit 1</t>
+  </si>
+  <si>
+    <t>SVMXC__Service_Order__c WO = new SVMXC__Service_Order__c ( SVMXC__Company__c = '001q000000kxZfw', SVMXC__Order_Status__c = 'Open' ,SVMXC__Country__c = 'United States', SVMXC__Sub_Status__c = 'Resolved', SVMXC__Priority__c = 'High');insert WO;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -189,12 +60,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF931A68"/>
-      <name val="Monaco"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Monaco"/>
     </font>
   </fonts>
@@ -218,9 +84,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -503,26 +372,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="110.83203125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="63.83203125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" ht="90" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 10125 and 10123.sah for SFM Search test cases and made changes to methods and objects
Added 10125 and 10123.sah for SFM Search test cases and made changes to methods and objects
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/backOffice/bo_excleData/SFMSearchDatasheet.xlsx
+++ b/svmx/test_lab/test_cases/backOffice/bo_excleData/SFMSearchDatasheet.xlsx
@@ -27,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>CreateWorkOrder</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>fetchwo</t>
   </si>
@@ -39,13 +36,22 @@
   </si>
   <si>
     <t>SVMXC__Service_Order__c WO = new SVMXC__Service_Order__c ( SVMXC__Company__c = '001q000000kxZfw', SVMXC__Order_Status__c = 'Open' ,SVMXC__Country__c = 'United States', SVMXC__Sub_Status__c = 'Resolved', SVMXC__Priority__c = 'High');insert WO;</t>
+  </si>
+  <si>
+    <t>CreateWorkOrderOpen</t>
+  </si>
+  <si>
+    <t>SVMXC__Service_Order__c WO = new SVMXC__Service_Order__c ( SVMXC__Company__c = '001q000000kxZfw', SVMXC__Order_Status__c = 'Canceled' ,SVMXC__Country__c = 'United States', SVMXC__Sub_Status__c = 'Resolved', SVMXC__Priority__c = 'High');insert WO;</t>
+  </si>
+  <si>
+    <t>CreateWorkOrderCanceled</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -62,6 +68,22 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Monaco"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -81,8 +103,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -96,7 +120,9 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -372,36 +398,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="110.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="63.83203125" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="61" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="90" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made changes to SFM Search test cases
Made changes to SFM Search test cases
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/backOffice/bo_excleData/SFMSearchDatasheet.xlsx
+++ b/svmx/test_lab/test_cases/backOffice/bo_excleData/SFMSearchDatasheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>fetchwo</t>
   </si>
@@ -45,6 +45,48 @@
   </si>
   <si>
     <t>CreateWorkOrderCanceled</t>
+  </si>
+  <si>
+    <t>CreateAccount</t>
+  </si>
+  <si>
+    <t>Account  acc = New Account(Name = 'Account Automation 1', Type = 'Analyst');insert acc ;</t>
+  </si>
+  <si>
+    <t>fetchaccount</t>
+  </si>
+  <si>
+    <t>Select Name , Id from Account where Name = 'Account Automation 1' AND Createdby.Id = '005q0000003GGfP' Order by CreatedDate DESC Limit 1</t>
+  </si>
+  <si>
+    <t>CreateServiceContract</t>
+  </si>
+  <si>
+    <t>FetchServiceContract</t>
+  </si>
+  <si>
+    <t>SVMXC__Service_Contract__c service_contract = New SVMXC__Service_Contract__c (Name = 'SCON RS_1022', SVMXC__Active__c = true , SVMXC__All_Contacts_Covered__c = true , SVMXC__Company__c = '001q000000kxZfw');insert service_contract;</t>
+  </si>
+  <si>
+    <t>Select Name , Id from SVMXC__Service_Contract__c where Name = 'SCON RS_1022' AND Createdby.Id = '005q0000003GGfP' Order by CreatedDate DESC Limit 1</t>
+  </si>
+  <si>
+    <t>SVMXC</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>001q000000kxZfw</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>005q0000003GGfP</t>
+  </si>
+  <si>
+    <t>OrgDetails</t>
   </si>
 </sst>
 </file>
@@ -103,12 +145,44 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -119,10 +193,45 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -398,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -409,10 +518,17 @@
     <col min="1" max="1" width="110.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="63.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="61" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="66" style="1" customWidth="1"/>
+    <col min="5" max="5" width="44.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="78.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="81.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="36.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="37.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="28.1640625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -422,8 +538,29 @@
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="90" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="90" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -432,6 +569,27 @@
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>